<commit_message>
Bug encontrado em que pula dois itens do Dropdown - Causa pode ser por causa do scroll que a página da automaticamente
</commit_message>
<xml_diff>
--- a/Base_Fipe.xlsx
+++ b/Base_Fipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.vinicius\Documents\Vscode\Fipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB13EB3-BC6C-4A51-8938-1ABD5AA311C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B663A440-00B6-4C0F-8035-9F521999DF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="22">
   <si>
     <t>Marca</t>
   </si>
@@ -43,28 +43,13 @@
     <t>Acura</t>
   </si>
   <si>
-    <t>Agrale</t>
-  </si>
-  <si>
-    <t>Alfa Romeo</t>
-  </si>
-  <si>
     <t>Integra GS 1.8</t>
   </si>
   <si>
     <t>Legend 3.2/3.5</t>
   </si>
   <si>
-    <t>MARRUÁ 2.8 12V 132cv TDI Diesel</t>
-  </si>
-  <si>
-    <t>MARRUÁ AM 100 2.8  CS TDI Diesel</t>
-  </si>
-  <si>
-    <t>145 Elegant 1.7/1.8 16V</t>
-  </si>
-  <si>
-    <t>145 Elegant 2.0 16V</t>
+    <t>NSX 3.0</t>
   </si>
   <si>
     <t>038003-2</t>
@@ -73,13 +58,7 @@
     <t>038002-4</t>
   </si>
   <si>
-    <t>060001-6</t>
-  </si>
-  <si>
-    <t>006009-7</t>
-  </si>
-  <si>
-    <t>006001-1</t>
+    <t>038001-6</t>
   </si>
   <si>
     <t>1992</t>
@@ -94,19 +73,19 @@
     <t>1997</t>
   </si>
   <si>
-    <t>2007</t>
-  </si>
-  <si>
-    <t>2006</t>
-  </si>
-  <si>
-    <t>1999</t>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>1993</t>
   </si>
   <si>
     <t>Gasolina</t>
-  </si>
-  <si>
-    <t>Diesel</t>
   </si>
 </sst>
 </file>
@@ -165,13 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,21 +453,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -515,243 +490,303 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>11097</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>10366</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>25397</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>22580</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>19084</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>14802</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>14219</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>14219</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>14219</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>14219</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2">
-        <v>11120</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>40991</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>39550</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>36538</v>
+      </c>
+      <c r="E14" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2">
-        <v>10387</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2">
-        <v>14248</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2">
-        <v>14248</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2">
-        <v>48348</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2">
-        <v>44601</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2">
-        <v>44601</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="D15">
+        <v>33397</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2">
-        <v>43449</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2">
-        <v>27043</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="2">
-        <v>21667</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="D16">
+        <v>33397</v>
+      </c>
+      <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2">
-        <v>21690</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="2">
-        <v>17716</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>27</v>
+      <c r="F16" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>